<commit_message>
added axis to graph
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="23040" windowHeight="9675"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="23040" windowHeight="9675"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1574,11 +1574,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="358509096"/>
-        <c:axId val="358509488"/>
+        <c:axId val="370456280"/>
+        <c:axId val="370456672"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="358509096"/>
+        <c:axId val="370456280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="27"/>
@@ -1611,6 +1611,65 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Correct Guesses per</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> 52 Cards</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1641,13 +1700,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="358509488"/>
+        <c:crossAx val="370456672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="358509488"/>
+        <c:axId val="370456672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.13"/>
@@ -1680,6 +1739,60 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Probability of Outcome</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.00%" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1710,7 +1823,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="358509096"/>
+        <c:crossAx val="370456280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1.0000000000000002E-2"/>
@@ -2389,13 +2502,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
+      <xdr:colOff>600076</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>476250</xdr:colOff>
+      <xdr:colOff>28576</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>161924</xdr:rowOff>
     </xdr:to>
@@ -2685,7 +2798,7 @@
   <dimension ref="A1:P54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="X9" sqref="X9"/>
+      <selection activeCell="T4" sqref="T4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>